<commit_message>
Fixed mistake in methanol inventory
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-lpg-from-methanol.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-lpg-from-methanol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4BFD75-92B7-4F8A-8685-E6FD15A1057C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEDC524-6640-48E7-91A0-550BEEA58270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9298BCFA-26D7-4294-BFA1-FE6048E95447}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{9298BCFA-26D7-4294-BFA1-FE6048E95447}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="84">
   <si>
     <t>Activity</t>
   </si>
@@ -212,12 +212,6 @@
     <t>Carbon monoxide, non-fossil</t>
   </si>
   <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
     <t>market group for electricity, low voltage</t>
   </si>
   <si>
@@ -280,11 +274,26 @@
   <si>
     <t>RAS</t>
   </si>
+  <si>
+    <t>Car db</t>
+  </si>
+  <si>
+    <t>market for water, ultrapure</t>
+  </si>
+  <si>
+    <t>water, ultrapure</t>
+  </si>
+  <si>
+    <t>CA-QC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -337,12 +346,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4674D2C-5661-4846-9F02-29F681DCA85F}">
   <dimension ref="A1:H643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A624" workbookViewId="0">
-      <selection activeCell="A628" sqref="A628"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -732,7 +742,7 @@
         <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -865,7 +875,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.13321500162583566</v>
@@ -986,13 +996,13 @@
         <v>52</v>
       </c>
       <c r="B29">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -1150,7 +1160,7 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1205,8 +1215,8 @@
         <v>21</v>
       </c>
       <c r="B45">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -1235,7 +1245,7 @@
         <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
@@ -1249,32 +1259,35 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B47" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C47" t="s">
+        <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G47" t="s">
+        <v>82</v>
       </c>
       <c r="H47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B48" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C48" t="s">
         <v>35</v>
@@ -1294,11 +1307,11 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B49" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C49" t="s">
         <v>35</v>
@@ -1310,7 +1323,7 @@
         <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H49" t="s">
         <v>32</v>
@@ -1318,11 +1331,11 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B50" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C50" t="s">
         <v>35</v>
@@ -1334,7 +1347,7 @@
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H50" t="s">
         <v>32</v>
@@ -1342,23 +1355,23 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" t="s">
         <v>66</v>
-      </c>
-      <c r="B51">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" t="s">
-        <v>68</v>
       </c>
       <c r="H51" t="s">
         <v>32</v>
@@ -1366,11 +1379,11 @@
     </row>
     <row r="52" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B52" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C52" t="s">
         <v>35</v>
@@ -1382,7 +1395,7 @@
         <v>15</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H52" t="s">
         <v>3</v>
@@ -1390,11 +1403,11 @@
     </row>
     <row r="53" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B53" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
@@ -1406,7 +1419,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H53" t="s">
         <v>3</v>
@@ -1457,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -1465,7 +1478,7 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -1515,7 +1528,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D65" t="s">
         <v>14</v>
@@ -1581,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
         <v>14</v>
@@ -1598,13 +1611,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B69">
         <v>0.13321500162583566</v>
       </c>
       <c r="C69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -1680,7 +1693,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -1719,13 +1732,13 @@
         <v>52</v>
       </c>
       <c r="B81">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F81" t="s">
         <v>15</v>
@@ -1745,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D82" t="s">
         <v>14</v>
@@ -1883,7 +1896,7 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -1899,7 +1912,7 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -1938,8 +1951,8 @@
         <v>21</v>
       </c>
       <c r="B97">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C97" t="s">
         <v>33</v>
@@ -1965,10 +1978,10 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F98" t="s">
         <v>22</v>
@@ -1982,35 +1995,38 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B99">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B99" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C99" t="s">
+        <v>55</v>
       </c>
       <c r="D99" t="s">
-        <v>43</v>
-      </c>
-      <c r="E99" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G99" t="s">
+        <v>82</v>
       </c>
       <c r="H99" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B100">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B100" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C100" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -2027,11 +2043,11 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>62</v>
-      </c>
-      <c r="B101">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B101" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C101" t="s">
         <v>35</v>
@@ -2043,7 +2059,7 @@
         <v>15</v>
       </c>
       <c r="G101" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H101" t="s">
         <v>32</v>
@@ -2051,11 +2067,11 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>64</v>
-      </c>
-      <c r="B102">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B102" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C102" t="s">
         <v>35</v>
@@ -2067,7 +2083,7 @@
         <v>15</v>
       </c>
       <c r="G102" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H102" t="s">
         <v>32</v>
@@ -2075,23 +2091,23 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>65</v>
+      </c>
+      <c r="D103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103" t="s">
         <v>66</v>
-      </c>
-      <c r="B103">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C103" t="s">
-        <v>67</v>
-      </c>
-      <c r="D103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" t="s">
-        <v>15</v>
-      </c>
-      <c r="G103" t="s">
-        <v>68</v>
       </c>
       <c r="H103" t="s">
         <v>32</v>
@@ -2099,14 +2115,14 @@
     </row>
     <row r="104" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B104">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B104" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C104" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D104" t="s">
         <v>14</v>
@@ -2115,7 +2131,7 @@
         <v>15</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H104" t="s">
         <v>3</v>
@@ -2123,11 +2139,11 @@
     </row>
     <row r="105" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B105">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B105" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C105" t="s">
         <v>33</v>
@@ -2139,7 +2155,7 @@
         <v>15</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H105" t="s">
         <v>3</v>
@@ -2190,7 +2206,7 @@
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
@@ -2198,7 +2214,7 @@
         <v>50</v>
       </c>
       <c r="B113" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
@@ -2248,7 +2264,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C117" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D117" t="s">
         <v>14</v>
@@ -2314,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D120" t="s">
         <v>14</v>
@@ -2331,13 +2347,13 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B121">
         <v>0.13321500162583566</v>
       </c>
       <c r="C121" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
@@ -2413,7 +2429,7 @@
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.35">
@@ -2452,13 +2468,13 @@
         <v>52</v>
       </c>
       <c r="B133">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D133" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F133" t="s">
         <v>15</v>
@@ -2478,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D134" t="s">
         <v>14</v>
@@ -2616,7 +2632,7 @@
         <v>6</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -2632,7 +2648,7 @@
         <v>11</v>
       </c>
       <c r="B146" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -2671,8 +2687,8 @@
         <v>21</v>
       </c>
       <c r="B149">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C149" t="s">
         <v>33</v>
@@ -2698,10 +2714,10 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D150" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F150" t="s">
         <v>22</v>
@@ -2715,35 +2731,38 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>59</v>
-      </c>
-      <c r="B151">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B151" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C151" t="s">
+        <v>55</v>
       </c>
       <c r="D151" t="s">
-        <v>43</v>
-      </c>
-      <c r="E151" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G151" t="s">
+        <v>82</v>
       </c>
       <c r="H151" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>61</v>
-      </c>
-      <c r="B152">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B152" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C152" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D152" t="s">
         <v>7</v>
@@ -2760,11 +2779,11 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>62</v>
-      </c>
-      <c r="B153">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B153" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C153" t="s">
         <v>35</v>
@@ -2776,7 +2795,7 @@
         <v>15</v>
       </c>
       <c r="G153" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H153" t="s">
         <v>32</v>
@@ -2784,11 +2803,11 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>64</v>
-      </c>
-      <c r="B154">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B154" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C154" t="s">
         <v>35</v>
@@ -2800,7 +2819,7 @@
         <v>15</v>
       </c>
       <c r="G154" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H154" t="s">
         <v>32</v>
@@ -2808,23 +2827,23 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>64</v>
+      </c>
+      <c r="B155" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C155" t="s">
+        <v>65</v>
+      </c>
+      <c r="D155" t="s">
+        <v>14</v>
+      </c>
+      <c r="F155" t="s">
+        <v>15</v>
+      </c>
+      <c r="G155" t="s">
         <v>66</v>
-      </c>
-      <c r="B155">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C155" t="s">
-        <v>67</v>
-      </c>
-      <c r="D155" t="s">
-        <v>14</v>
-      </c>
-      <c r="F155" t="s">
-        <v>15</v>
-      </c>
-      <c r="G155" t="s">
-        <v>68</v>
       </c>
       <c r="H155" t="s">
         <v>32</v>
@@ -2832,14 +2851,14 @@
     </row>
     <row r="156" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B156">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B156" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C156" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D156" t="s">
         <v>14</v>
@@ -2848,7 +2867,7 @@
         <v>15</v>
       </c>
       <c r="G156" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H156" t="s">
         <v>3</v>
@@ -2856,11 +2875,11 @@
     </row>
     <row r="157" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B157">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B157" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C157" t="s">
         <v>33</v>
@@ -2872,7 +2891,7 @@
         <v>15</v>
       </c>
       <c r="G157" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H157" t="s">
         <v>3</v>
@@ -2923,7 +2942,7 @@
         <v>11</v>
       </c>
       <c r="B164" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -2931,7 +2950,7 @@
         <v>50</v>
       </c>
       <c r="B165" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
@@ -2981,7 +3000,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C169" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D169" t="s">
         <v>14</v>
@@ -3047,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="C172" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D172" t="s">
         <v>14</v>
@@ -3064,13 +3083,13 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B173">
         <v>0.13321500162583566</v>
       </c>
       <c r="C173" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D173" t="s">
         <v>7</v>
@@ -3146,7 +3165,7 @@
         <v>11</v>
       </c>
       <c r="B182" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -3185,13 +3204,13 @@
         <v>52</v>
       </c>
       <c r="B185">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D185" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F185" t="s">
         <v>15</v>
@@ -3211,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D186" t="s">
         <v>14</v>
@@ -3349,7 +3368,7 @@
         <v>6</v>
       </c>
       <c r="B196" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
@@ -3365,7 +3384,7 @@
         <v>11</v>
       </c>
       <c r="B198" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -3404,8 +3423,8 @@
         <v>21</v>
       </c>
       <c r="B201">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C201" t="s">
         <v>33</v>
@@ -3431,10 +3450,10 @@
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D202" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F202" t="s">
         <v>22</v>
@@ -3448,35 +3467,38 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>59</v>
-      </c>
-      <c r="B203">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B203" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C203" t="s">
+        <v>55</v>
       </c>
       <c r="D203" t="s">
-        <v>43</v>
-      </c>
-      <c r="E203" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F203" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G203" t="s">
+        <v>82</v>
       </c>
       <c r="H203" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>61</v>
-      </c>
-      <c r="B204">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B204" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C204" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D204" t="s">
         <v>7</v>
@@ -3493,11 +3515,11 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>62</v>
-      </c>
-      <c r="B205">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B205" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C205" t="s">
         <v>35</v>
@@ -3509,7 +3531,7 @@
         <v>15</v>
       </c>
       <c r="G205" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H205" t="s">
         <v>32</v>
@@ -3517,11 +3539,11 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>64</v>
-      </c>
-      <c r="B206">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B206" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C206" t="s">
         <v>35</v>
@@ -3533,7 +3555,7 @@
         <v>15</v>
       </c>
       <c r="G206" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H206" t="s">
         <v>32</v>
@@ -3541,23 +3563,23 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
+        <v>64</v>
+      </c>
+      <c r="B207" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>65</v>
+      </c>
+      <c r="D207" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" t="s">
+        <v>15</v>
+      </c>
+      <c r="G207" t="s">
         <v>66</v>
-      </c>
-      <c r="B207">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C207" t="s">
-        <v>67</v>
-      </c>
-      <c r="D207" t="s">
-        <v>14</v>
-      </c>
-      <c r="F207" t="s">
-        <v>15</v>
-      </c>
-      <c r="G207" t="s">
-        <v>68</v>
       </c>
       <c r="H207" t="s">
         <v>32</v>
@@ -3565,14 +3587,14 @@
     </row>
     <row r="208" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A208" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B208">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B208" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C208" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D208" t="s">
         <v>14</v>
@@ -3581,7 +3603,7 @@
         <v>15</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H208" t="s">
         <v>3</v>
@@ -3589,11 +3611,11 @@
     </row>
     <row r="209" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A209" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B209">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B209" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C209" t="s">
         <v>33</v>
@@ -3605,7 +3627,7 @@
         <v>15</v>
       </c>
       <c r="G209" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H209" t="s">
         <v>3</v>
@@ -3656,7 +3678,7 @@
         <v>11</v>
       </c>
       <c r="B216" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.35">
@@ -3664,7 +3686,7 @@
         <v>50</v>
       </c>
       <c r="B217" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.35">
@@ -3714,7 +3736,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C221" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D221" t="s">
         <v>14</v>
@@ -3780,7 +3802,7 @@
         <v>1</v>
       </c>
       <c r="C224" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D224" t="s">
         <v>14</v>
@@ -3797,13 +3819,13 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B225">
         <v>0.13321500162583566</v>
       </c>
       <c r="C225" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D225" t="s">
         <v>7</v>
@@ -3879,7 +3901,7 @@
         <v>11</v>
       </c>
       <c r="B234" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.35">
@@ -3918,13 +3940,13 @@
         <v>52</v>
       </c>
       <c r="B237">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C237" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D237" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F237" t="s">
         <v>15</v>
@@ -3944,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="C238" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D238" t="s">
         <v>14</v>
@@ -4082,7 +4104,7 @@
         <v>6</v>
       </c>
       <c r="B248" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.35">
@@ -4098,7 +4120,7 @@
         <v>11</v>
       </c>
       <c r="B250" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -4137,8 +4159,8 @@
         <v>21</v>
       </c>
       <c r="B253">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C253" t="s">
         <v>33</v>
@@ -4164,10 +4186,10 @@
         <v>1</v>
       </c>
       <c r="C254" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D254" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F254" t="s">
         <v>22</v>
@@ -4181,35 +4203,38 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>59</v>
-      </c>
-      <c r="B255">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B255" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C255" t="s">
+        <v>55</v>
       </c>
       <c r="D255" t="s">
-        <v>43</v>
-      </c>
-      <c r="E255" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F255" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G255" t="s">
+        <v>82</v>
       </c>
       <c r="H255" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>61</v>
-      </c>
-      <c r="B256">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B256" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C256" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D256" t="s">
         <v>7</v>
@@ -4226,11 +4251,11 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>62</v>
-      </c>
-      <c r="B257">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B257" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C257" t="s">
         <v>35</v>
@@ -4242,7 +4267,7 @@
         <v>15</v>
       </c>
       <c r="G257" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H257" t="s">
         <v>32</v>
@@ -4250,11 +4275,11 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>64</v>
-      </c>
-      <c r="B258">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B258" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C258" t="s">
         <v>35</v>
@@ -4266,7 +4291,7 @@
         <v>15</v>
       </c>
       <c r="G258" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H258" t="s">
         <v>32</v>
@@ -4274,23 +4299,23 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
+        <v>64</v>
+      </c>
+      <c r="B259" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C259" t="s">
+        <v>65</v>
+      </c>
+      <c r="D259" t="s">
+        <v>14</v>
+      </c>
+      <c r="F259" t="s">
+        <v>15</v>
+      </c>
+      <c r="G259" t="s">
         <v>66</v>
-      </c>
-      <c r="B259">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C259" t="s">
-        <v>67</v>
-      </c>
-      <c r="D259" t="s">
-        <v>14</v>
-      </c>
-      <c r="F259" t="s">
-        <v>15</v>
-      </c>
-      <c r="G259" t="s">
-        <v>68</v>
       </c>
       <c r="H259" t="s">
         <v>32</v>
@@ -4298,14 +4323,14 @@
     </row>
     <row r="260" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A260" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B260">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B260" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C260" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D260" t="s">
         <v>14</v>
@@ -4314,7 +4339,7 @@
         <v>15</v>
       </c>
       <c r="G260" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H260" t="s">
         <v>3</v>
@@ -4322,11 +4347,11 @@
     </row>
     <row r="261" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A261" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B261">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B261" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C261" t="s">
         <v>33</v>
@@ -4338,7 +4363,7 @@
         <v>15</v>
       </c>
       <c r="G261" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H261" t="s">
         <v>3</v>
@@ -4389,7 +4414,7 @@
         <v>11</v>
       </c>
       <c r="B268" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.35">
@@ -4397,7 +4422,7 @@
         <v>50</v>
       </c>
       <c r="B269" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.35">
@@ -4447,7 +4472,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C273" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D273" t="s">
         <v>14</v>
@@ -4513,7 +4538,7 @@
         <v>1</v>
       </c>
       <c r="C276" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D276" t="s">
         <v>14</v>
@@ -4536,7 +4561,7 @@
         <v>0.13321500162583566</v>
       </c>
       <c r="C277" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D277" t="s">
         <v>7</v>
@@ -4612,7 +4637,7 @@
         <v>11</v>
       </c>
       <c r="B286" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.35">
@@ -4651,13 +4676,13 @@
         <v>52</v>
       </c>
       <c r="B289">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C289" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D289" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F289" t="s">
         <v>15</v>
@@ -4677,7 +4702,7 @@
         <v>1</v>
       </c>
       <c r="C290" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D290" t="s">
         <v>14</v>
@@ -4815,7 +4840,7 @@
         <v>6</v>
       </c>
       <c r="B300" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.35">
@@ -4831,7 +4856,7 @@
         <v>11</v>
       </c>
       <c r="B302" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="303" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -4870,8 +4895,8 @@
         <v>21</v>
       </c>
       <c r="B305">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C305" t="s">
         <v>33</v>
@@ -4897,10 +4922,10 @@
         <v>1</v>
       </c>
       <c r="C306" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D306" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F306" t="s">
         <v>22</v>
@@ -4914,35 +4939,38 @@
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>59</v>
-      </c>
-      <c r="B307">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B307" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C307" t="s">
+        <v>55</v>
       </c>
       <c r="D307" t="s">
-        <v>43</v>
-      </c>
-      <c r="E307" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F307" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G307" t="s">
+        <v>82</v>
       </c>
       <c r="H307" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>23</v>
-      </c>
-      <c r="B308">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B308" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C308" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D308" t="s">
         <v>7</v>
@@ -4959,11 +4987,11 @@
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>62</v>
-      </c>
-      <c r="B309">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B309" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C309" t="s">
         <v>35</v>
@@ -4975,7 +5003,7 @@
         <v>15</v>
       </c>
       <c r="G309" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H309" t="s">
         <v>32</v>
@@ -4983,11 +5011,11 @@
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>64</v>
-      </c>
-      <c r="B310">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B310" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C310" t="s">
         <v>35</v>
@@ -4999,7 +5027,7 @@
         <v>15</v>
       </c>
       <c r="G310" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H310" t="s">
         <v>32</v>
@@ -5007,23 +5035,23 @@
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
+        <v>64</v>
+      </c>
+      <c r="B311" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C311" t="s">
+        <v>65</v>
+      </c>
+      <c r="D311" t="s">
+        <v>14</v>
+      </c>
+      <c r="F311" t="s">
+        <v>15</v>
+      </c>
+      <c r="G311" t="s">
         <v>66</v>
-      </c>
-      <c r="B311">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C311" t="s">
-        <v>67</v>
-      </c>
-      <c r="D311" t="s">
-        <v>14</v>
-      </c>
-      <c r="F311" t="s">
-        <v>15</v>
-      </c>
-      <c r="G311" t="s">
-        <v>68</v>
       </c>
       <c r="H311" t="s">
         <v>32</v>
@@ -5031,14 +5059,14 @@
     </row>
     <row r="312" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A312" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B312">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B312" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C312" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D312" t="s">
         <v>14</v>
@@ -5047,7 +5075,7 @@
         <v>15</v>
       </c>
       <c r="G312" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H312" t="s">
         <v>3</v>
@@ -5055,11 +5083,11 @@
     </row>
     <row r="313" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A313" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B313">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B313" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C313" t="s">
         <v>33</v>
@@ -5071,7 +5099,7 @@
         <v>15</v>
       </c>
       <c r="G313" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H313" t="s">
         <v>3</v>
@@ -5122,7 +5150,7 @@
         <v>11</v>
       </c>
       <c r="B320" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.35">
@@ -5130,7 +5158,7 @@
         <v>50</v>
       </c>
       <c r="B321" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.35">
@@ -5180,7 +5208,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C325" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D325" t="s">
         <v>14</v>
@@ -5246,7 +5274,7 @@
         <v>1</v>
       </c>
       <c r="C328" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D328" t="s">
         <v>14</v>
@@ -5269,7 +5297,7 @@
         <v>0.13321500162583566</v>
       </c>
       <c r="C329" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D329" t="s">
         <v>7</v>
@@ -5345,7 +5373,7 @@
         <v>11</v>
       </c>
       <c r="B338" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.35">
@@ -5384,13 +5412,13 @@
         <v>52</v>
       </c>
       <c r="B341">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C341" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D341" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F341" t="s">
         <v>15</v>
@@ -5410,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="C342" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D342" t="s">
         <v>14</v>
@@ -5548,7 +5576,7 @@
         <v>6</v>
       </c>
       <c r="B352" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.35">
@@ -5564,7 +5592,7 @@
         <v>11</v>
       </c>
       <c r="B354" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="355" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -5603,8 +5631,8 @@
         <v>21</v>
       </c>
       <c r="B357">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C357" t="s">
         <v>33</v>
@@ -5630,10 +5658,10 @@
         <v>1</v>
       </c>
       <c r="C358" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D358" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F358" t="s">
         <v>22</v>
@@ -5647,35 +5675,38 @@
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>59</v>
-      </c>
-      <c r="B359">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B359" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C359" t="s">
+        <v>55</v>
       </c>
       <c r="D359" t="s">
-        <v>43</v>
-      </c>
-      <c r="E359" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F359" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G359" t="s">
+        <v>82</v>
       </c>
       <c r="H359" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>23</v>
-      </c>
-      <c r="B360">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B360" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C360" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D360" t="s">
         <v>7</v>
@@ -5692,11 +5723,11 @@
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>62</v>
-      </c>
-      <c r="B361">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B361" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C361" t="s">
         <v>35</v>
@@ -5708,7 +5739,7 @@
         <v>15</v>
       </c>
       <c r="G361" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H361" t="s">
         <v>32</v>
@@ -5716,11 +5747,11 @@
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>64</v>
-      </c>
-      <c r="B362">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B362" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C362" t="s">
         <v>35</v>
@@ -5732,7 +5763,7 @@
         <v>15</v>
       </c>
       <c r="G362" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H362" t="s">
         <v>32</v>
@@ -5740,23 +5771,23 @@
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
+        <v>64</v>
+      </c>
+      <c r="B363" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C363" t="s">
+        <v>65</v>
+      </c>
+      <c r="D363" t="s">
+        <v>14</v>
+      </c>
+      <c r="F363" t="s">
+        <v>15</v>
+      </c>
+      <c r="G363" t="s">
         <v>66</v>
-      </c>
-      <c r="B363">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C363" t="s">
-        <v>67</v>
-      </c>
-      <c r="D363" t="s">
-        <v>14</v>
-      </c>
-      <c r="F363" t="s">
-        <v>15</v>
-      </c>
-      <c r="G363" t="s">
-        <v>68</v>
       </c>
       <c r="H363" t="s">
         <v>32</v>
@@ -5764,14 +5795,14 @@
     </row>
     <row r="364" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A364" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B364">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B364" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C364" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D364" t="s">
         <v>14</v>
@@ -5780,7 +5811,7 @@
         <v>15</v>
       </c>
       <c r="G364" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H364" t="s">
         <v>3</v>
@@ -5788,11 +5819,11 @@
     </row>
     <row r="365" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A365" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B365">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B365" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C365" t="s">
         <v>33</v>
@@ -5804,7 +5835,7 @@
         <v>15</v>
       </c>
       <c r="G365" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H365" t="s">
         <v>3</v>
@@ -5855,7 +5886,7 @@
         <v>11</v>
       </c>
       <c r="B372" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="373" spans="1:8" x14ac:dyDescent="0.35">
@@ -5863,7 +5894,7 @@
         <v>50</v>
       </c>
       <c r="B373" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="374" spans="1:8" x14ac:dyDescent="0.35">
@@ -5913,7 +5944,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C377" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D377" t="s">
         <v>14</v>
@@ -5979,7 +6010,7 @@
         <v>1</v>
       </c>
       <c r="C380" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D380" t="s">
         <v>14</v>
@@ -5996,13 +6027,13 @@
     </row>
     <row r="381" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B381">
         <v>0.13321500162583566</v>
       </c>
       <c r="C381" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D381" t="s">
         <v>7</v>
@@ -6078,7 +6109,7 @@
         <v>11</v>
       </c>
       <c r="B390" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="391" spans="1:8" x14ac:dyDescent="0.35">
@@ -6117,13 +6148,13 @@
         <v>52</v>
       </c>
       <c r="B393">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C393" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D393" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F393" t="s">
         <v>15</v>
@@ -6143,7 +6174,7 @@
         <v>1</v>
       </c>
       <c r="C394" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D394" t="s">
         <v>14</v>
@@ -6281,7 +6312,7 @@
         <v>6</v>
       </c>
       <c r="B404" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.35">
@@ -6297,7 +6328,7 @@
         <v>11</v>
       </c>
       <c r="B406" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="407" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -6336,8 +6367,8 @@
         <v>21</v>
       </c>
       <c r="B409">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C409" t="s">
         <v>33</v>
@@ -6363,10 +6394,10 @@
         <v>1</v>
       </c>
       <c r="C410" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D410" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F410" t="s">
         <v>22</v>
@@ -6380,35 +6411,38 @@
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>59</v>
-      </c>
-      <c r="B411">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B411" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C411" t="s">
+        <v>83</v>
       </c>
       <c r="D411" t="s">
-        <v>43</v>
-      </c>
-      <c r="E411" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F411" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G411" t="s">
+        <v>82</v>
       </c>
       <c r="H411" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>61</v>
-      </c>
-      <c r="B412">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B412" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C412" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D412" t="s">
         <v>7</v>
@@ -6425,11 +6459,11 @@
     </row>
     <row r="413" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>62</v>
-      </c>
-      <c r="B413">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B413" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C413" t="s">
         <v>35</v>
@@ -6441,7 +6475,7 @@
         <v>15</v>
       </c>
       <c r="G413" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H413" t="s">
         <v>32</v>
@@ -6449,11 +6483,11 @@
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>64</v>
-      </c>
-      <c r="B414">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B414" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C414" t="s">
         <v>35</v>
@@ -6465,7 +6499,7 @@
         <v>15</v>
       </c>
       <c r="G414" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H414" t="s">
         <v>32</v>
@@ -6473,23 +6507,23 @@
     </row>
     <row r="415" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
+        <v>64</v>
+      </c>
+      <c r="B415" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C415" t="s">
+        <v>65</v>
+      </c>
+      <c r="D415" t="s">
+        <v>14</v>
+      </c>
+      <c r="F415" t="s">
+        <v>15</v>
+      </c>
+      <c r="G415" t="s">
         <v>66</v>
-      </c>
-      <c r="B415">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C415" t="s">
-        <v>67</v>
-      </c>
-      <c r="D415" t="s">
-        <v>14</v>
-      </c>
-      <c r="F415" t="s">
-        <v>15</v>
-      </c>
-      <c r="G415" t="s">
-        <v>68</v>
       </c>
       <c r="H415" t="s">
         <v>32</v>
@@ -6497,14 +6531,14 @@
     </row>
     <row r="416" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A416" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B416">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B416" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C416" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D416" t="s">
         <v>14</v>
@@ -6513,7 +6547,7 @@
         <v>15</v>
       </c>
       <c r="G416" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H416" t="s">
         <v>3</v>
@@ -6521,11 +6555,11 @@
     </row>
     <row r="417" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A417" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B417">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B417" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C417" t="s">
         <v>33</v>
@@ -6537,7 +6571,7 @@
         <v>15</v>
       </c>
       <c r="G417" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H417" t="s">
         <v>3</v>
@@ -6588,7 +6622,7 @@
         <v>11</v>
       </c>
       <c r="B424" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.35">
@@ -6596,7 +6630,7 @@
         <v>50</v>
       </c>
       <c r="B425" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.35">
@@ -6646,7 +6680,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C429" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D429" t="s">
         <v>14</v>
@@ -6712,7 +6746,7 @@
         <v>1</v>
       </c>
       <c r="C432" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D432" t="s">
         <v>14</v>
@@ -6729,13 +6763,13 @@
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B433">
         <v>0.13321500162583566</v>
       </c>
       <c r="C433" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D433" t="s">
         <v>7</v>
@@ -6811,7 +6845,7 @@
         <v>11</v>
       </c>
       <c r="B442" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.35">
@@ -6850,13 +6884,13 @@
         <v>52</v>
       </c>
       <c r="B445">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C445" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D445" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F445" t="s">
         <v>15</v>
@@ -6876,7 +6910,7 @@
         <v>1</v>
       </c>
       <c r="C446" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D446" t="s">
         <v>14</v>
@@ -7014,7 +7048,7 @@
         <v>6</v>
       </c>
       <c r="B456" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.35">
@@ -7030,7 +7064,7 @@
         <v>11</v>
       </c>
       <c r="B458" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="459" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -7069,8 +7103,8 @@
         <v>21</v>
       </c>
       <c r="B461">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C461" t="s">
         <v>33</v>
@@ -7096,10 +7130,10 @@
         <v>1</v>
       </c>
       <c r="C462" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D462" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F462" t="s">
         <v>22</v>
@@ -7113,35 +7147,38 @@
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>59</v>
-      </c>
-      <c r="B463">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B463" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C463" t="s">
+        <v>55</v>
       </c>
       <c r="D463" t="s">
-        <v>43</v>
-      </c>
-      <c r="E463" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F463" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G463" t="s">
+        <v>82</v>
       </c>
       <c r="H463" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>61</v>
-      </c>
-      <c r="B464">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B464" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C464" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D464" t="s">
         <v>7</v>
@@ -7158,11 +7195,11 @@
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>62</v>
-      </c>
-      <c r="B465">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B465" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C465" t="s">
         <v>35</v>
@@ -7174,7 +7211,7 @@
         <v>15</v>
       </c>
       <c r="G465" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H465" t="s">
         <v>32</v>
@@ -7182,11 +7219,11 @@
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>64</v>
-      </c>
-      <c r="B466">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B466" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C466" t="s">
         <v>35</v>
@@ -7198,7 +7235,7 @@
         <v>15</v>
       </c>
       <c r="G466" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H466" t="s">
         <v>32</v>
@@ -7206,23 +7243,23 @@
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
+        <v>64</v>
+      </c>
+      <c r="B467" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C467" t="s">
+        <v>65</v>
+      </c>
+      <c r="D467" t="s">
+        <v>14</v>
+      </c>
+      <c r="F467" t="s">
+        <v>15</v>
+      </c>
+      <c r="G467" t="s">
         <v>66</v>
-      </c>
-      <c r="B467">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C467" t="s">
-        <v>67</v>
-      </c>
-      <c r="D467" t="s">
-        <v>14</v>
-      </c>
-      <c r="F467" t="s">
-        <v>15</v>
-      </c>
-      <c r="G467" t="s">
-        <v>68</v>
       </c>
       <c r="H467" t="s">
         <v>32</v>
@@ -7230,14 +7267,14 @@
     </row>
     <row r="468" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A468" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B468">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B468" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C468" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D468" t="s">
         <v>14</v>
@@ -7246,7 +7283,7 @@
         <v>15</v>
       </c>
       <c r="G468" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H468" t="s">
         <v>3</v>
@@ -7254,11 +7291,11 @@
     </row>
     <row r="469" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A469" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B469">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B469" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C469" t="s">
         <v>33</v>
@@ -7270,7 +7307,7 @@
         <v>15</v>
       </c>
       <c r="G469" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H469" t="s">
         <v>3</v>
@@ -7321,7 +7358,7 @@
         <v>11</v>
       </c>
       <c r="B476" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="477" spans="1:8" x14ac:dyDescent="0.35">
@@ -7329,7 +7366,7 @@
         <v>50</v>
       </c>
       <c r="B477" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="478" spans="1:8" x14ac:dyDescent="0.35">
@@ -7379,7 +7416,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C481" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D481" t="s">
         <v>14</v>
@@ -7445,7 +7482,7 @@
         <v>1</v>
       </c>
       <c r="C484" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D484" t="s">
         <v>14</v>
@@ -7462,13 +7499,13 @@
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B485">
         <v>0.13321500162583566</v>
       </c>
       <c r="C485" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D485" t="s">
         <v>7</v>
@@ -7544,7 +7581,7 @@
         <v>11</v>
       </c>
       <c r="B494" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.35">
@@ -7583,13 +7620,13 @@
         <v>52</v>
       </c>
       <c r="B497">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C497" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D497" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F497" t="s">
         <v>15</v>
@@ -7609,7 +7646,7 @@
         <v>1</v>
       </c>
       <c r="C498" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D498" t="s">
         <v>14</v>
@@ -7747,7 +7784,7 @@
         <v>6</v>
       </c>
       <c r="B508" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="509" spans="1:8" x14ac:dyDescent="0.35">
@@ -7763,7 +7800,7 @@
         <v>11</v>
       </c>
       <c r="B510" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="511" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -7802,8 +7839,8 @@
         <v>21</v>
       </c>
       <c r="B513">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C513" t="s">
         <v>33</v>
@@ -7829,10 +7866,10 @@
         <v>1</v>
       </c>
       <c r="C514" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D514" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F514" t="s">
         <v>22</v>
@@ -7846,35 +7883,38 @@
     </row>
     <row r="515" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
-        <v>59</v>
-      </c>
-      <c r="B515">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B515" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C515" t="s">
+        <v>55</v>
       </c>
       <c r="D515" t="s">
-        <v>43</v>
-      </c>
-      <c r="E515" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F515" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G515" t="s">
+        <v>82</v>
       </c>
       <c r="H515" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>61</v>
-      </c>
-      <c r="B516">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B516" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C516" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D516" t="s">
         <v>7</v>
@@ -7891,11 +7931,11 @@
     </row>
     <row r="517" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>62</v>
-      </c>
-      <c r="B517">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B517" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C517" t="s">
         <v>35</v>
@@ -7907,7 +7947,7 @@
         <v>15</v>
       </c>
       <c r="G517" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H517" t="s">
         <v>32</v>
@@ -7915,11 +7955,11 @@
     </row>
     <row r="518" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>64</v>
-      </c>
-      <c r="B518">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B518" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C518" t="s">
         <v>35</v>
@@ -7931,7 +7971,7 @@
         <v>15</v>
       </c>
       <c r="G518" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H518" t="s">
         <v>32</v>
@@ -7939,23 +7979,23 @@
     </row>
     <row r="519" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
+        <v>64</v>
+      </c>
+      <c r="B519" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C519" t="s">
+        <v>65</v>
+      </c>
+      <c r="D519" t="s">
+        <v>14</v>
+      </c>
+      <c r="F519" t="s">
+        <v>15</v>
+      </c>
+      <c r="G519" t="s">
         <v>66</v>
-      </c>
-      <c r="B519">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C519" t="s">
-        <v>67</v>
-      </c>
-      <c r="D519" t="s">
-        <v>14</v>
-      </c>
-      <c r="F519" t="s">
-        <v>15</v>
-      </c>
-      <c r="G519" t="s">
-        <v>68</v>
       </c>
       <c r="H519" t="s">
         <v>32</v>
@@ -7963,14 +8003,14 @@
     </row>
     <row r="520" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A520" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B520">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B520" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C520" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D520" t="s">
         <v>14</v>
@@ -7979,7 +8019,7 @@
         <v>15</v>
       </c>
       <c r="G520" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H520" t="s">
         <v>3</v>
@@ -7987,11 +8027,11 @@
     </row>
     <row r="521" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A521" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B521">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B521" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C521" t="s">
         <v>33</v>
@@ -8003,7 +8043,7 @@
         <v>15</v>
       </c>
       <c r="G521" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H521" t="s">
         <v>3</v>
@@ -8054,7 +8094,7 @@
         <v>11</v>
       </c>
       <c r="B528" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="529" spans="1:8" x14ac:dyDescent="0.35">
@@ -8062,7 +8102,7 @@
         <v>50</v>
       </c>
       <c r="B529" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="530" spans="1:8" x14ac:dyDescent="0.35">
@@ -8112,7 +8152,7 @@
         <v>2.2053430633360036</v>
       </c>
       <c r="C533" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D533" t="s">
         <v>14</v>
@@ -8178,7 +8218,7 @@
         <v>1</v>
       </c>
       <c r="C536" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D536" t="s">
         <v>14</v>
@@ -8195,13 +8235,13 @@
     </row>
     <row r="537" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B537">
         <v>0.13321500162583566</v>
       </c>
       <c r="C537" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D537" t="s">
         <v>7</v>
@@ -8277,7 +8317,7 @@
         <v>11</v>
       </c>
       <c r="B546" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="547" spans="1:8" x14ac:dyDescent="0.35">
@@ -8316,13 +8356,13 @@
         <v>52</v>
       </c>
       <c r="B549">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C549" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D549" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F549" t="s">
         <v>15</v>
@@ -8342,7 +8382,7 @@
         <v>1</v>
       </c>
       <c r="C550" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D550" t="s">
         <v>14</v>
@@ -8480,7 +8520,7 @@
         <v>6</v>
       </c>
       <c r="B560" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="561" spans="1:8" x14ac:dyDescent="0.35">
@@ -8496,7 +8536,7 @@
         <v>11</v>
       </c>
       <c r="B562" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="563" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -8535,8 +8575,8 @@
         <v>21</v>
       </c>
       <c r="B565">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C565" t="s">
         <v>33</v>
@@ -8562,10 +8602,10 @@
         <v>1</v>
       </c>
       <c r="C566" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D566" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F566" t="s">
         <v>22</v>
@@ -8579,35 +8619,38 @@
     </row>
     <row r="567" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>59</v>
-      </c>
-      <c r="B567">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+        <v>81</v>
+      </c>
+      <c r="B567" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
+      </c>
+      <c r="C567" t="s">
+        <v>55</v>
       </c>
       <c r="D567" t="s">
-        <v>43</v>
-      </c>
-      <c r="E567" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F567" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G567" t="s">
+        <v>82</v>
       </c>
       <c r="H567" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="568" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>61</v>
-      </c>
-      <c r="B568">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
+        <v>59</v>
+      </c>
+      <c r="B568" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
       </c>
       <c r="C568" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D568" t="s">
         <v>7</v>
@@ -8624,11 +8667,11 @@
     </row>
     <row r="569" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>62</v>
-      </c>
-      <c r="B569">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+        <v>60</v>
+      </c>
+      <c r="B569" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
       </c>
       <c r="C569" t="s">
         <v>35</v>
@@ -8640,7 +8683,7 @@
         <v>15</v>
       </c>
       <c r="G569" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H569" t="s">
         <v>32</v>
@@ -8648,11 +8691,11 @@
     </row>
     <row r="570" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>64</v>
-      </c>
-      <c r="B570">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+        <v>62</v>
+      </c>
+      <c r="B570" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C570" t="s">
         <v>35</v>
@@ -8664,7 +8707,7 @@
         <v>15</v>
       </c>
       <c r="G570" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H570" t="s">
         <v>32</v>
@@ -8672,23 +8715,23 @@
     </row>
     <row r="571" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
+        <v>64</v>
+      </c>
+      <c r="B571" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
+      </c>
+      <c r="C571" t="s">
+        <v>65</v>
+      </c>
+      <c r="D571" t="s">
+        <v>14</v>
+      </c>
+      <c r="F571" t="s">
+        <v>15</v>
+      </c>
+      <c r="G571" t="s">
         <v>66</v>
-      </c>
-      <c r="B571">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
-      </c>
-      <c r="C571" t="s">
-        <v>67</v>
-      </c>
-      <c r="D571" t="s">
-        <v>14</v>
-      </c>
-      <c r="F571" t="s">
-        <v>15</v>
-      </c>
-      <c r="G571" t="s">
-        <v>68</v>
       </c>
       <c r="H571" t="s">
         <v>32</v>
@@ -8696,14 +8739,14 @@
     </row>
     <row r="572" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A572" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B572">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>67</v>
+      </c>
+      <c r="B572" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C572" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D572" t="s">
         <v>14</v>
@@ -8712,7 +8755,7 @@
         <v>15</v>
       </c>
       <c r="G572" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H572" t="s">
         <v>3</v>
@@ -8720,11 +8763,11 @@
     </row>
     <row r="573" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A573" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B573">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
+        <v>68</v>
+      </c>
+      <c r="B573" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C573" t="s">
         <v>33</v>
@@ -8736,7 +8779,7 @@
         <v>15</v>
       </c>
       <c r="G573" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H573" t="s">
         <v>3</v>
@@ -8795,7 +8838,7 @@
         <v>50</v>
       </c>
       <c r="B581" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.35">
@@ -8928,7 +8971,7 @@
     </row>
     <row r="589" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B589">
         <v>0.13321500162583566</v>
@@ -9049,13 +9092,13 @@
         <v>52</v>
       </c>
       <c r="B601">
-        <v>5.5277777777777777</v>
+        <v>1</v>
       </c>
       <c r="C601" t="s">
         <v>33</v>
       </c>
       <c r="D601" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F601" t="s">
         <v>15</v>
@@ -9213,143 +9256,162 @@
         <v>6</v>
       </c>
       <c r="B612" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A613" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B613" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="614" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A614" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="614" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A614" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="615" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A615" t="s">
+        <v>9</v>
+      </c>
+      <c r="B615" t="s">
+        <v>10</v>
+      </c>
+      <c r="C615" t="s">
         <v>11</v>
       </c>
-      <c r="B614" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="615" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A615" s="1" t="s">
-        <v>8</v>
+      <c r="D615" t="s">
+        <v>6</v>
+      </c>
+      <c r="E615" t="s">
+        <v>12</v>
+      </c>
+      <c r="F615" t="s">
+        <v>4</v>
+      </c>
+      <c r="G615" t="s">
+        <v>2</v>
+      </c>
+      <c r="H615" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="616" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A616" t="s">
-        <v>9</v>
-      </c>
-      <c r="B616" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B616">
+        <f>12.89</f>
+        <v>12.89</v>
       </c>
       <c r="C616" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D616" t="s">
         <v>6</v>
       </c>
-      <c r="E616" t="s">
-        <v>12</v>
-      </c>
       <c r="F616" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G616" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H616" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
     </row>
     <row r="617" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A617" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B617">
-        <f>12.89/5.72</f>
-        <v>2.2534965034965038</v>
+        <v>1</v>
       </c>
       <c r="C617" t="s">
         <v>33</v>
       </c>
       <c r="D617" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F617" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G617" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H617" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="618" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A618" t="s">
-        <v>52</v>
-      </c>
-      <c r="B618">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="B618" s="5">
+        <f>((3090000*1000)/44900000)</f>
+        <v>68.819599109131403</v>
       </c>
       <c r="C618" t="s">
         <v>33</v>
       </c>
       <c r="D618" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F618" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G618" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="H618" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="619" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A619" t="s">
         <v>59</v>
       </c>
-      <c r="B619">
-        <f>3090000/44900000/5.472</f>
-        <v>1.2576681123744774E-2</v>
+      <c r="B619" s="5">
+        <f>(13600*1000)/44900000</f>
+        <v>0.30289532293986637</v>
+      </c>
+      <c r="C619" t="s">
+        <v>33</v>
       </c>
       <c r="D619" t="s">
-        <v>43</v>
-      </c>
-      <c r="E619" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="F619" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G619" t="s">
+        <v>25</v>
       </c>
       <c r="H619" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="620" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A620" t="s">
+        <v>60</v>
+      </c>
+      <c r="B620" s="5">
+        <f>356/44900000</f>
+        <v>7.9287305122494425E-6</v>
+      </c>
+      <c r="C620" t="s">
+        <v>35</v>
+      </c>
+      <c r="D620" t="s">
+        <v>14</v>
+      </c>
+      <c r="F620" t="s">
+        <v>15</v>
+      </c>
+      <c r="G620" t="s">
         <v>61</v>
-      </c>
-      <c r="B620">
-        <f>13600000/44900000/5.472</f>
-        <v>5.5353677437841073E-2</v>
-      </c>
-      <c r="C620" t="s">
-        <v>33</v>
-      </c>
-      <c r="D620" t="s">
-        <v>7</v>
-      </c>
-      <c r="F620" t="s">
-        <v>15</v>
-      </c>
-      <c r="G620" t="s">
-        <v>25</v>
       </c>
       <c r="H620" t="s">
         <v>32</v>
@@ -9359,9 +9421,9 @@
       <c r="A621" t="s">
         <v>62</v>
       </c>
-      <c r="B621">
-        <f>356/44900000/5.472</f>
-        <v>1.4489639094023102E-6</v>
+      <c r="B621" s="5">
+        <f>949/44900000</f>
+        <v>2.11358574610245E-5</v>
       </c>
       <c r="C621" t="s">
         <v>35</v>
@@ -9383,12 +9445,12 @@
       <c r="A622" t="s">
         <v>64</v>
       </c>
-      <c r="B622">
-        <f>949/44900000/5.472</f>
-        <v>3.8625470506258219E-6</v>
+      <c r="B622" s="5">
+        <f>178/44900000</f>
+        <v>3.9643652561247212E-6</v>
       </c>
       <c r="C622" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D622" t="s">
         <v>14</v>
@@ -9397,43 +9459,43 @@
         <v>15</v>
       </c>
       <c r="G622" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H622" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A623" t="s">
-        <v>66</v>
-      </c>
-      <c r="B623">
-        <f>178/44900000/5.472</f>
-        <v>7.2448195470115511E-7</v>
+    <row r="623" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A623" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B623" s="5">
+        <f>6240000/44900000</f>
+        <v>0.13897550111358575</v>
       </c>
       <c r="C623" t="s">
+        <v>33</v>
+      </c>
+      <c r="D623" t="s">
+        <v>14</v>
+      </c>
+      <c r="F623" t="s">
+        <v>15</v>
+      </c>
+      <c r="G623" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D623" t="s">
-        <v>14</v>
-      </c>
-      <c r="F623" t="s">
-        <v>15</v>
-      </c>
-      <c r="G623" t="s">
-        <v>68</v>
-      </c>
       <c r="H623" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="624" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A624" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B624">
-        <f>(6240000/44900000/42/5.472)*0.09</f>
-        <v>5.4423363531322738E-5</v>
+        <v>68</v>
+      </c>
+      <c r="B624" s="5">
+        <f>75900000/44900000</f>
+        <v>1.6904231625835189</v>
       </c>
       <c r="C624" t="s">
         <v>33</v>
@@ -9445,35 +9507,15 @@
         <v>15</v>
       </c>
       <c r="G624" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H624" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="625" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A625" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B625">
-        <f>75900000/44900000/5.472</f>
-        <v>0.30892236158324538</v>
-      </c>
-      <c r="C625" t="s">
-        <v>33</v>
-      </c>
-      <c r="D625" t="s">
-        <v>14</v>
-      </c>
-      <c r="F625" t="s">
-        <v>15</v>
-      </c>
-      <c r="G625" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H625" t="s">
-        <v>3</v>
-      </c>
+      <c r="A625" s="4"/>
+      <c r="G625" s="4"/>
     </row>
     <row r="627" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A627" s="1" t="s">

</xml_diff>

<commit_message>
Updated Readme and other fixes
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-lpg-from-methanol.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-lpg-from-methanol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEDC524-6640-48E7-91A0-550BEEA58270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F139BC-465F-456D-9969-25677CB48987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{9298BCFA-26D7-4294-BFA1-FE6048E95447}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9298BCFA-26D7-4294-BFA1-FE6048E95447}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4674D2C-5661-4846-9F02-29F681DCA85F}">
   <dimension ref="A1:H643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B308" s="5">
         <f>(13600*1000)/44900000</f>
@@ -5699,7 +5699,7 @@
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B360" s="5">
         <f>(13600*1000)/44900000</f>

</xml_diff>